<commit_message>
added sql db connection
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -29,13 +29,19 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
+    <t xml:space="preserve">adminadmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emre@Furkan28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin1</t>
   </si>
 </sst>
 </file>
@@ -45,11 +51,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -65,6 +72,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,8 +123,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,29 +261,32 @@
   </sheetPr>
   <dimension ref="A2:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="Emre@Furkan28"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -279,33 +304,33 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>